<commit_message>
Confirmed the features that I plan to implement.
</commit_message>
<xml_diff>
--- a/Features Roadmap.xlsx
+++ b/Features Roadmap.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Caleb\Desktop\Easy Artistry\EasyArtistry\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\osullc2\Desktop\School\S24\RCOS\EasyArtistry\EasyArtistry\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B232AEA6-3657-4E59-AFB7-565A74817F3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16771EA3-92A4-4882-83F8-7AFC802E7BD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="14592" xr2:uid="{1D6ACA5A-D6F5-4BD0-A0C8-51F0E3FEBB6A}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" xr2:uid="{1D6ACA5A-D6F5-4BD0-A0C8-51F0E3FEBB6A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="28">
   <si>
     <t>Feature</t>
   </si>
@@ -117,6 +117,9 @@
   </si>
   <si>
     <t>Impliment GUI Mockup</t>
+  </si>
+  <si>
+    <t>Colin</t>
   </si>
 </sst>
 </file>
@@ -549,7 +552,7 @@
   <dimension ref="B2:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -721,7 +724,7 @@
         <v>15</v>
       </c>
       <c r="C11" t="s">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="D11" t="s">
         <v>6</v>
@@ -736,7 +739,7 @@
         <v>16</v>
       </c>
       <c r="C12" t="s">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="D12" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
Determined which features to implement
</commit_message>
<xml_diff>
--- a/Features Roadmap.xlsx
+++ b/Features Roadmap.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\osullc2\Desktop\School\S24\RCOS\EasyArtistry\EasyArtistry\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Easy_Artistry_tutorials\EasyArtistry\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16771EA3-92A4-4882-83F8-7AFC802E7BD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{047D7CFD-1063-43EA-9274-27D0B829C705}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" xr2:uid="{1D6ACA5A-D6F5-4BD0-A0C8-51F0E3FEBB6A}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{1D6ACA5A-D6F5-4BD0-A0C8-51F0E3FEBB6A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="29">
   <si>
     <t>Feature</t>
   </si>
@@ -120,6 +120,9 @@
   </si>
   <si>
     <t>Colin</t>
+  </si>
+  <si>
+    <t>Annabelle</t>
   </si>
 </sst>
 </file>
@@ -552,19 +555,19 @@
   <dimension ref="B2:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="32.1015625" customWidth="1"/>
-    <col min="3" max="3" width="21.89453125" customWidth="1"/>
-    <col min="4" max="4" width="20.9453125" customWidth="1"/>
-    <col min="5" max="5" width="20.05078125" customWidth="1"/>
-    <col min="8" max="8" width="27.578125" customWidth="1"/>
+    <col min="2" max="2" width="32.08984375" customWidth="1"/>
+    <col min="3" max="3" width="21.90625" customWidth="1"/>
+    <col min="4" max="4" width="20.90625" customWidth="1"/>
+    <col min="5" max="5" width="20.08984375" customWidth="1"/>
+    <col min="8" max="8" width="27.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -584,7 +587,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>4</v>
       </c>
@@ -602,7 +605,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>8</v>
       </c>
@@ -620,7 +623,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>9</v>
       </c>
@@ -638,7 +641,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>18</v>
       </c>
@@ -656,7 +659,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>11</v>
       </c>
@@ -674,7 +677,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>12</v>
       </c>
@@ -689,12 +692,12 @@
       </c>
       <c r="F8" s="3"/>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
         <v>13</v>
       </c>
       <c r="C9" t="s">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="D9" t="s">
         <v>6</v>
@@ -704,12 +707,12 @@
       </c>
       <c r="F9" s="3"/>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>14</v>
       </c>
       <c r="C10" t="s">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="D10" t="s">
         <v>6</v>
@@ -719,7 +722,7 @@
       </c>
       <c r="F10" s="3"/>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>15</v>
       </c>
@@ -734,7 +737,7 @@
       </c>
       <c r="F11" s="4"/>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
         <v>16</v>
       </c>
@@ -749,7 +752,7 @@
       </c>
       <c r="F12" s="5"/>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
         <v>17</v>
       </c>
@@ -764,7 +767,7 @@
       </c>
       <c r="F13" s="3"/>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
         <v>19</v>
       </c>
@@ -779,7 +782,7 @@
       </c>
       <c r="F14" s="2"/>
     </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
         <v>26</v>
       </c>

</xml_diff>

<commit_message>
Confirmed which features I plan to implement
</commit_message>
<xml_diff>
--- a/Features Roadmap.xlsx
+++ b/Features Roadmap.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\osullc2\Desktop\School\S24\RCOS\EasyArtistry\EasyArtistry\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\first_commit_easy_artistry\EasyArtistry\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16771EA3-92A4-4882-83F8-7AFC802E7BD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CF21087-D472-42AC-A85C-49D169668E08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" xr2:uid="{1D6ACA5A-D6F5-4BD0-A0C8-51F0E3FEBB6A}"/>
+    <workbookView xWindow="930" yWindow="530" windowWidth="9140" windowHeight="9550" xr2:uid="{1D6ACA5A-D6F5-4BD0-A0C8-51F0E3FEBB6A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="29">
   <si>
     <t>Feature</t>
   </si>
@@ -120,6 +120,9 @@
   </si>
   <si>
     <t>Colin</t>
+  </si>
+  <si>
+    <t>Annabelle</t>
   </si>
 </sst>
 </file>
@@ -552,19 +555,19 @@
   <dimension ref="B2:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="32.1015625" customWidth="1"/>
-    <col min="3" max="3" width="21.89453125" customWidth="1"/>
-    <col min="4" max="4" width="20.9453125" customWidth="1"/>
-    <col min="5" max="5" width="20.05078125" customWidth="1"/>
-    <col min="8" max="8" width="27.578125" customWidth="1"/>
+    <col min="2" max="2" width="32.08984375" customWidth="1"/>
+    <col min="3" max="3" width="21.90625" customWidth="1"/>
+    <col min="4" max="4" width="20.90625" customWidth="1"/>
+    <col min="5" max="5" width="20.08984375" customWidth="1"/>
+    <col min="8" max="8" width="27.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -584,7 +587,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>4</v>
       </c>
@@ -602,7 +605,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>8</v>
       </c>
@@ -620,7 +623,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>9</v>
       </c>
@@ -638,7 +641,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>18</v>
       </c>
@@ -656,7 +659,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>11</v>
       </c>
@@ -674,7 +677,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>12</v>
       </c>
@@ -689,12 +692,12 @@
       </c>
       <c r="F8" s="3"/>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
         <v>13</v>
       </c>
       <c r="C9" t="s">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="D9" t="s">
         <v>6</v>
@@ -704,12 +707,12 @@
       </c>
       <c r="F9" s="3"/>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>14</v>
       </c>
       <c r="C10" t="s">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="D10" t="s">
         <v>6</v>
@@ -719,7 +722,7 @@
       </c>
       <c r="F10" s="3"/>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>15</v>
       </c>
@@ -734,7 +737,7 @@
       </c>
       <c r="F11" s="4"/>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
         <v>16</v>
       </c>
@@ -749,7 +752,7 @@
       </c>
       <c r="F12" s="5"/>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
         <v>17</v>
       </c>
@@ -764,7 +767,7 @@
       </c>
       <c r="F13" s="3"/>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
         <v>19</v>
       </c>
@@ -779,7 +782,7 @@
       </c>
       <c r="F14" s="2"/>
     </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
         <v>26</v>
       </c>

</xml_diff>

<commit_message>
things i plan to work on
</commit_message>
<xml_diff>
--- a/Features Roadmap.xlsx
+++ b/Features Roadmap.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\first_commit_easy_artistry\EasyArtistry\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sebastian Grammas\Dropbox\RCOS\EasyArtistry\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FC1A4D3-8332-4B8C-9E6E-95CC2E9BBDFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AEEFE0C-F107-4993-A526-CFCDE7919D02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="930" yWindow="530" windowWidth="9140" windowHeight="9550" xr2:uid="{1D6ACA5A-D6F5-4BD0-A0C8-51F0E3FEBB6A}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{1D6ACA5A-D6F5-4BD0-A0C8-51F0E3FEBB6A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="30">
   <si>
     <t>Feature</t>
   </si>
@@ -123,6 +123,9 @@
   </si>
   <si>
     <t>Annabelle</t>
+  </si>
+  <si>
+    <t>Sebastian</t>
   </si>
 </sst>
 </file>
@@ -555,7 +558,7 @@
   <dimension ref="B2:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -610,7 +613,7 @@
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="D4" t="s">
         <v>6</v>
@@ -757,7 +760,7 @@
         <v>17</v>
       </c>
       <c r="C13" t="s">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="D13" t="s">
         <v>6</v>

</xml_diff>